<commit_message>
Finished opcode in deicmal and binary.
</commit_message>
<xml_diff>
--- a/assign_1_ops.xlsx
+++ b/assign_1_ops.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne\Dropbox\College\Current\Arch\Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne\Dropbox\College\Current\Arch\Projects\Project_1\CS3339\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FEF428-DEB0-4FF4-843F-C29C303970D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD7C7CB-569A-4601-A8DF-0B78733841B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18744" windowHeight="12624" xr2:uid="{3B3B85E7-C9DA-452D-AF06-8A1A44E04738}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
   <si>
     <t>ADD</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Rt</t>
+  </si>
+  <si>
+    <t>dec</t>
+  </si>
+  <si>
+    <t>bin</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -243,6 +249,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -252,7 +261,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -569,29 +587,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1ACAC51-A77F-4BA0-91AC-4CBF423A522F}">
-  <dimension ref="B2:H49"/>
+  <dimension ref="B2:H64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="6.109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="15.44140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -620,10 +639,10 @@
       <c r="D5" s="1">
         <v>11</v>
       </c>
-      <c r="E5" s="9">
-        <v>5</v>
-      </c>
-      <c r="F5" s="9">
+      <c r="E5" s="6">
+        <v>5</v>
+      </c>
+      <c r="F5" s="6">
         <v>6</v>
       </c>
       <c r="G5" s="1">
@@ -633,244 +652,485 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1112</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1">
+        <v>10001011000</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1">
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
-        <v>12</v>
+      <c r="C10" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="D10" s="1">
-        <v>11</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="G11" s="9"/>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1">
+        <v>11001011000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D13" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1691</v>
+      </c>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1">
+        <v>11010011011</v>
+      </c>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="1">
+        <v>11010011010</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="1">
+      <c r="C21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="1" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="1">
+        <v>10001010000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="1">
+      <c r="C25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="1">
+        <v>10101010000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="1">
+      <c r="C29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C31" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="1">
+        <v>11001010000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="2"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D27" s="1" t="s">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E35" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="1" t="s">
+      <c r="F35" s="12"/>
+      <c r="G35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
+      <c r="H35" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="1">
+      <c r="C36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="1">
         <v>10</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E36" s="10">
         <v>12</v>
       </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="1">
-        <v>5</v>
-      </c>
-      <c r="H28" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="8"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>26</v>
+      <c r="F36" s="12"/>
+      <c r="G36" s="1">
+        <v>5</v>
+      </c>
+      <c r="H36" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="1" t="s">
-        <v>18</v>
+      <c r="C37" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="D37" s="1">
-        <v>11</v>
-      </c>
-      <c r="E37" s="1">
-        <v>9</v>
-      </c>
-      <c r="F37" s="1">
-        <v>2</v>
-      </c>
-      <c r="G37" s="1">
-        <v>5</v>
-      </c>
-      <c r="H37" s="1">
-        <v>5</v>
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C38" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="1">
+        <v>10010001000</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C41" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C42" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="1">
+        <v>11010001000</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="2"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="9"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="1">
+        <v>11</v>
+      </c>
+      <c r="E47" s="1">
+        <v>9</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2</v>
+      </c>
+      <c r="G47" s="1">
+        <v>5</v>
+      </c>
+      <c r="H47" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D48" s="1">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D49" s="1">
+        <v>11111000010</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B51" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D51" s="1">
         <v>11</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E51" s="1">
         <v>9</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F51" s="1">
         <v>2</v>
       </c>
-      <c r="G40" s="1">
-        <v>5</v>
-      </c>
-      <c r="H40" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="6" t="s">
+      <c r="G51" s="1">
+        <v>5</v>
+      </c>
+      <c r="H51" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D52" s="1">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D53" s="1">
+        <v>11111000000</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B54" s="2"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B55" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="8"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D45" s="1" t="s">
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="9"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D57" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E57" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F45" s="3"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="1" t="s">
+      <c r="F57" s="11"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="1" t="s">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B58" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D58" s="1">
         <v>8</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E58" s="10">
         <v>19</v>
       </c>
-      <c r="F46" s="3"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="1" t="s">
+      <c r="F58" s="11"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D59" s="1">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D60" s="1">
+        <v>10110100111</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B62" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D62" s="1">
         <v>8</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E62" s="10">
         <v>19</v>
       </c>
-      <c r="F49" s="3"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="1">
-        <v>5</v>
+      <c r="F62" s="11"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D63" s="1">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D64" s="1">
+        <v>10110101000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B2:H2"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="B55:H55"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B33:H33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
gimme my files this time
</commit_message>
<xml_diff>
--- a/assign_1_ops.xlsx
+++ b/assign_1_ops.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne\Dropbox\College\Current\Arch\Projects\Project_1\CS3339\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne\Dropbox\College\Current\Arch\Projects\All_Project_1\Project_1\CS3339\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD7C7CB-569A-4601-A8DF-0B78733841B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8640280-CF7A-4F10-A945-524EF0DF8D4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18744" windowHeight="12624" xr2:uid="{3B3B85E7-C9DA-452D-AF06-8A1A44E04738}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
   <si>
     <t>ADD</t>
   </si>
@@ -117,6 +117,78 @@
   </si>
   <si>
     <t>bin</t>
+  </si>
+  <si>
+    <t>IM-Formats</t>
+  </si>
+  <si>
+    <t>MOVK</t>
+  </si>
+  <si>
+    <t>1940 - 1943</t>
+  </si>
+  <si>
+    <t>11110010100 - 11110010111</t>
+  </si>
+  <si>
+    <t>MOVZ</t>
+  </si>
+  <si>
+    <t>1684 - 1687</t>
+  </si>
+  <si>
+    <t>11010010100 - 11010010111</t>
+  </si>
+  <si>
+    <t>1160 - 1161</t>
+  </si>
+  <si>
+    <t>10010001000 - 10010001001</t>
+  </si>
+  <si>
+    <t>1672 - 1673</t>
+  </si>
+  <si>
+    <t>11010001000 - 11010001001</t>
+  </si>
+  <si>
+    <t>1440 - 1447</t>
+  </si>
+  <si>
+    <t>10110100000 - 10110100111</t>
+  </si>
+  <si>
+    <t>1448 - 1455</t>
+  </si>
+  <si>
+    <t>10110101000 - 10110101111</t>
+  </si>
+  <si>
+    <t>B-Formats</t>
+  </si>
+  <si>
+    <t>160 - 191</t>
+  </si>
+  <si>
+    <t>10100000 - 10111111</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>00000000000</t>
+  </si>
+  <si>
+    <t>MISC-Formats</t>
   </si>
 </sst>
 </file>
@@ -168,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -206,17 +278,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1" tint="0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color theme="1" tint="0.24994659260841701"/>
       </right>
@@ -232,8 +293,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -243,34 +325,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -587,17 +642,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1ACAC51-A77F-4BA0-91AC-4CBF423A522F}">
-  <dimension ref="B2:H64"/>
+  <dimension ref="B2:H105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="6.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -605,17 +660,14 @@
       <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
@@ -633,16 +685,16 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1">
         <v>11</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
         <v>5</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="3">
         <v>6</v>
       </c>
       <c r="G5" s="1">
@@ -653,38 +705,38 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1">
         <v>1112</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1">
         <v>10001011000</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="1">
@@ -692,445 +744,549 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="1">
         <v>11001011000</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C12" s="5"/>
-    </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="1">
         <v>1691</v>
       </c>
-      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="1">
         <v>11010011011</v>
       </c>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G16" s="3"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="1">
         <v>1690</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C19" s="5" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="1">
         <v>11010011010</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="1">
         <v>1104</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C23" s="5" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="1">
         <v>10001010000</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="1">
         <v>1360</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C27" s="5" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C27" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="1">
         <v>10101010000</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="1">
         <v>1616</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C31" s="5" t="s">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="1">
         <v>11001010000</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="7" t="s">
+    <row r="32" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="2"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="9"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D35" s="1" t="s">
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D39" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E39" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="1" t="s">
+      <c r="F39" s="8"/>
+      <c r="G39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="1">
-        <v>10</v>
-      </c>
-      <c r="E36" s="10">
-        <v>12</v>
-      </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="1">
-        <v>5</v>
-      </c>
-      <c r="H36" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C37" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1160</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C38" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="1">
-        <v>10010001000</v>
-      </c>
-    </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="1">
         <v>10</v>
       </c>
+      <c r="E40" s="8">
+        <v>12</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" s="1">
+        <v>5</v>
+      </c>
+      <c r="H40" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C41" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1672</v>
-      </c>
+      <c r="C41" s="2"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C42" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D42" s="1">
-        <v>11010001000</v>
+      <c r="B42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="2"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="7" t="s">
+      <c r="C43" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="9"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D46" s="1" t="s">
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D51" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="1">
-        <v>11</v>
-      </c>
-      <c r="E47" s="1">
-        <v>9</v>
-      </c>
-      <c r="F47" s="1">
-        <v>2</v>
-      </c>
-      <c r="G47" s="1">
-        <v>5</v>
-      </c>
-      <c r="H47" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D48" s="1">
-        <v>1986</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D49" s="1">
-        <v>11111000010</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B51" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D51" s="1">
-        <v>11</v>
-      </c>
-      <c r="E51" s="1">
-        <v>9</v>
-      </c>
-      <c r="F51" s="1">
-        <v>2</v>
-      </c>
-      <c r="G51" s="1">
-        <v>5</v>
-      </c>
-      <c r="H51" s="1">
-        <v>5</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D52" s="1">
+        <v>11</v>
+      </c>
+      <c r="E52" s="1">
+        <v>9</v>
+      </c>
+      <c r="F52" s="1">
+        <v>2</v>
+      </c>
+      <c r="G52" s="1">
+        <v>5</v>
+      </c>
+      <c r="H52" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55" s="1">
+        <v>11111000010</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="1">
         <v>1984</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D53" s="1">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58" s="1">
         <v>11111000000</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B54" s="2"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B55" s="7" t="s">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B61" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="9"/>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D57" s="1" t="s">
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D63" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E63" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F57" s="11"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="1" t="s">
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B58" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D58" s="1">
-        <v>8</v>
-      </c>
-      <c r="E58" s="10">
-        <v>19</v>
-      </c>
-      <c r="F58" s="11"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D59" s="1">
-        <v>1447</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D60" s="1">
-        <v>10110100111</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D62" s="1">
-        <v>8</v>
-      </c>
-      <c r="E62" s="10">
-        <v>19</v>
-      </c>
-      <c r="F62" s="11"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D63" s="1">
-        <v>1448</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D64" s="1">
-        <v>10110101000</v>
-      </c>
-    </row>
+        <v>8</v>
+      </c>
+      <c r="E64" s="8">
+        <v>19</v>
+      </c>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B66" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C67" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B69" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C70" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B74" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G76" s="10"/>
+      <c r="H76" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D77" s="1">
+        <v>9</v>
+      </c>
+      <c r="E77" s="1">
+        <v>2</v>
+      </c>
+      <c r="F77" s="9">
+        <v>16</v>
+      </c>
+      <c r="G77" s="10"/>
+      <c r="H77" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B79" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C80" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B83" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C84" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D90" s="1">
+        <v>6</v>
+      </c>
+      <c r="E90" s="8">
+        <v>26</v>
+      </c>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="8"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B92" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C93" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B98" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D98" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B99" s="6"/>
+      <c r="C99" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="B74:H74"/>
+    <mergeCell ref="E89:H89"/>
+    <mergeCell ref="E90:H90"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F77:G77"/>
     <mergeCell ref="B2:H2"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="B55:H55"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="B37:H37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>